<commit_message>
Drools integrated and running code
</commit_message>
<xml_diff>
--- a/src/main/resources/com.livelabdrools.rule/rule.xlsx
+++ b/src/main/resources/com.livelabdrools.rule/rule.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitworkspace\arch_change\livelabdrools_poc\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitworkspace\arch_change\livelabdrools_poc\src\main\resources\com.livelabdrools.rule\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>RuleSet</t>
   </si>
   <si>
-    <t>rules</t>
-  </si>
-  <si>
     <t>Import</t>
   </si>
   <si>
@@ -120,15 +117,28 @@
   </si>
   <si>
     <t>com.livelabdrools.model.Person</t>
+  </si>
+  <si>
+    <t>"true"</t>
+  </si>
+  <si>
+    <t>com.livelabdrools</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -155,8 +165,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,7 +481,7 @@
   <dimension ref="B2:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,137 +496,137 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
         <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>